<commit_message>
implement data driven testing in login page
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/DemoDDT.xlsx
+++ b/src/test/resources/testData/DemoDDT.xlsx
@@ -13,29 +13,29 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>usename</t>
+    <t>Username</t>
   </si>
   <si>
     <t>password</t>
   </si>
   <si>
-    <t>usename 1</t>
-  </si>
-  <si>
-    <t>password 1</t>
-  </si>
-  <si>
-    <t>usename 2</t>
-  </si>
-  <si>
-    <t>password 2</t>
+    <t>QualityWay</t>
+  </si>
+  <si>
+    <t>pwd_ds_algo@2</t>
+  </si>
+  <si>
+    <t>QualityWayInvalid</t>
+  </si>
+  <si>
+    <t>pwd_ds_algo@2Invalid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -45,15 +45,28 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <color rgb="FF3F7F5F"/>
+      <name val="Consolas"/>
+    </font>
+    <font>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8F2FE"/>
+        <bgColor rgb="FFE8F2FE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,12 +75,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -294,18 +316,18 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>